<commit_message>
Version 3.3 Incluido -R
</commit_message>
<xml_diff>
--- a/tools/db/TEST.xlsx
+++ b/tools/db/TEST.xlsx
@@ -669,7 +669,7 @@
       </c>
       <c r="F1" s="1">
         <f>SUM(C2:C93)</f>
-        <v>5996</v>
+        <v>6231</v>
       </c>
     </row>
     <row ht="14.25" r="2">
@@ -1630,13 +1630,37 @@
       </c>
     </row>
     <row ht="14.25" r="89">
-      <c r="A89" s="2"/>
+      <c r="A89" s="2">
+        <v>16</v>
+      </c>
+      <c r="B89" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C89" s="0">
+        <v>80</v>
+      </c>
     </row>
     <row ht="14.25" r="90">
-      <c r="A90" s="2"/>
+      <c r="A90" s="2">
+        <v>19</v>
+      </c>
+      <c r="B90" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C90" s="0">
+        <v>80</v>
+      </c>
     </row>
     <row ht="14.25" r="91">
-      <c r="A91" s="2"/>
+      <c r="A91" s="2">
+        <v>24</v>
+      </c>
+      <c r="B91" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C91" s="0">
+        <v>75</v>
+      </c>
     </row>
     <row ht="14.25" r="92">
       <c r="A92" s="2"/>
@@ -1648,7 +1672,7 @@
       </c>
       <c r="C94" s="1">
         <f>SUM(C2:C93)</f>
-        <v>5996</v>
+        <v>6231</v>
       </c>
     </row>
     <row ht="14.25" r="95"/>

</xml_diff>